<commit_message>
fix time_alive data quality issue
</commit_message>
<xml_diff>
--- a/Blog Post Data Analysis/Model_Summary_2v2_V1.xlsx
+++ b/Blog Post Data Analysis/Model_Summary_2v2_V1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="222">
   <si>
     <t>Categorical Variable</t>
   </si>
@@ -149,6 +149,12 @@
     <t>N/A</t>
   </si>
   <si>
+    <t>Reduced Model</t>
+  </si>
+  <si>
+    <t>p value &gt; alpha and beta changes all less than 20%</t>
+  </si>
+  <si>
     <t>Order</t>
   </si>
   <si>
@@ -164,13 +170,13 @@
     <t>Linear</t>
   </si>
   <si>
-    <t>-34057.4853</t>
+    <t>-35450.3887</t>
   </si>
   <si>
     <t>First Order</t>
   </si>
   <si>
-    <t>-34151.9905</t>
+    <t>-35582.1406</t>
   </si>
   <si>
     <t>1.0</t>
@@ -182,100 +188,85 @@
     <t>Second Order</t>
   </si>
   <si>
-    <t>-34052.9861</t>
-  </si>
-  <si>
-    <t>0.0027</t>
-  </si>
-  <si>
-    <t>-34051.9737</t>
-  </si>
-  <si>
-    <t>0.3634</t>
-  </si>
-  <si>
-    <t>3, 1</t>
-  </si>
-  <si>
-    <t>-35403.4099</t>
+    <t>-36886.2623</t>
   </si>
   <si>
     <t>-1</t>
   </si>
   <si>
-    <t>-34097.0115</t>
-  </si>
-  <si>
-    <t>-34088.1402</t>
+    <t>-35440.119</t>
+  </si>
+  <si>
+    <t>&lt;0.0001</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>-34033.4352</t>
-  </si>
-  <si>
-    <t>&lt;0.0001</t>
-  </si>
-  <si>
-    <t>-34003.9528</t>
+    <t>-35416.4074</t>
+  </si>
+  <si>
+    <t>2, 3</t>
+  </si>
+  <si>
+    <t>-35468.3085</t>
+  </si>
+  <si>
+    <t>-35400.2746</t>
+  </si>
+  <si>
+    <t>-35382.9638</t>
   </si>
   <si>
     <t>0.5, 1</t>
   </si>
   <si>
-    <t>-34007.8743</t>
-  </si>
-  <si>
-    <t>-33998.5763</t>
-  </si>
-  <si>
-    <t>0.0001</t>
+    <t>-35386.8097</t>
+  </si>
+  <si>
+    <t>-35368.4357</t>
   </si>
   <si>
     <t>3, 2</t>
   </si>
   <si>
-    <t>-34052.434</t>
-  </si>
-  <si>
-    <t>0.0015</t>
-  </si>
-  <si>
-    <t>-33990.3493</t>
-  </si>
-  <si>
-    <t>-33968.6145</t>
-  </si>
-  <si>
-    <t>-33751.7223</t>
-  </si>
-  <si>
-    <t>-35416.5142</t>
-  </si>
-  <si>
-    <t>-34505.2259</t>
-  </si>
-  <si>
-    <t>-36958.0157</t>
-  </si>
-  <si>
-    <t>Received_-1</t>
-  </si>
-  <si>
-    <t>-33718.2571</t>
-  </si>
-  <si>
-    <t>-33744.9823</t>
-  </si>
-  <si>
-    <t>1, 0.5</t>
-  </si>
-  <si>
-    <t>-31770.2998</t>
-  </si>
-  <si>
-    <t>-30178.7411</t>
+    <t>-35424.7368</t>
+  </si>
+  <si>
+    <t>-35362.1289</t>
+  </si>
+  <si>
+    <t>2, 1</t>
+  </si>
+  <si>
+    <t>-35356.7095</t>
+  </si>
+  <si>
+    <t>-35167.4338</t>
+  </si>
+  <si>
+    <t>-37186.3657</t>
+  </si>
+  <si>
+    <t>-35819.8088</t>
+  </si>
+  <si>
+    <t>-38490.3186</t>
+  </si>
+  <si>
+    <t>-35675.444</t>
+  </si>
+  <si>
+    <t>-35520.7588</t>
+  </si>
+  <si>
+    <t>-2</t>
+  </si>
+  <si>
+    <t>-32506.636</t>
+  </si>
+  <si>
+    <t>-30427.1282</t>
   </si>
   <si>
     <t>1, 2</t>
@@ -284,7 +275,7 @@
     <t>Transformations</t>
   </si>
   <si>
-    <t>NetEnergyShards_3</t>
+    <t>Ultimates_2 | Ultimates_3</t>
   </si>
   <si>
     <t>Num_EX1_0.5 | Num_EX1_1</t>
@@ -293,15 +284,12 @@
     <t>Num_EX2_3 | Num_EX2_2</t>
   </si>
   <si>
-    <t>Control_Received_3 | Control_Received_1</t>
+    <t>Control_Received_2 | Control_Received_1</t>
   </si>
   <si>
     <t>Control_0.5 | Control_1</t>
   </si>
   <si>
-    <t>Ping_-1</t>
-  </si>
-  <si>
     <t>ScorePerSecond_1 | ScorePerSecond_2</t>
   </si>
   <si>
@@ -317,13 +305,19 @@
     <t>TeamRatioUltimatesAll20 x EnemyRatioUltimatesAll20</t>
   </si>
   <si>
-    <t>TeamRatioUltimatesAll20_TeamRatioREX50</t>
-  </si>
-  <si>
-    <t>TeamRatioUltimatesAll20 x TeamRatioREX50</t>
-  </si>
-  <si>
-    <t>TeamRatioUltimatesAll20_Ultimates</t>
+    <t>TeamRatioUltimatesAll20_NetHealthShards</t>
+  </si>
+  <si>
+    <t>TeamRatioUltimatesAll20 x NetHealthShards</t>
+  </si>
+  <si>
+    <t>TeamRatioUltimatesAll20_NetOrbs</t>
+  </si>
+  <si>
+    <t>TeamRatioUltimatesAll20 x NetOrbs</t>
+  </si>
+  <si>
+    <t>TeamRatioUltimatesAll20_Ultimates_2 | TeamRatioUltimatesAll20_Ultimates_3</t>
   </si>
   <si>
     <t>TeamRatioUltimatesAll20 x Ultimates</t>
@@ -335,19 +329,31 @@
     <t>TeamRatioUltimatesAll20 x Num_R</t>
   </si>
   <si>
+    <t>TeamRatioUltimatesAll20_Num_EX1_0.5 | TeamRatioUltimatesAll20_Num_EX1_1</t>
+  </si>
+  <si>
+    <t>TeamRatioUltimatesAll20 x Num_EX1</t>
+  </si>
+  <si>
     <t>TeamRatioUltimatesAll20_Num_EX2_3 | TeamRatioUltimatesAll20_Num_EX2_2</t>
   </si>
   <si>
     <t>TeamRatioUltimatesAll20 x Num_EX2</t>
   </si>
   <si>
-    <t>EnemyRatioUltimatesAll20_TeamRatioREX50</t>
-  </si>
-  <si>
-    <t>EnemyRatioUltimatesAll20 x TeamRatioREX50</t>
-  </si>
-  <si>
-    <t>EnemyRatioUltimatesAll20_Control_Received_3 | EnemyRatioUltimatesAll20_Control_Received_1</t>
+    <t>TeamRatioUltimatesAll20_Damage_Received</t>
+  </si>
+  <si>
+    <t>TeamRatioUltimatesAll20 x Damage_Received</t>
+  </si>
+  <si>
+    <t>EnemyRatioUltimatesAll20_Num_EX2_3 | EnemyRatioUltimatesAll20_Num_EX2_2</t>
+  </si>
+  <si>
+    <t>EnemyRatioUltimatesAll20 x Num_EX2</t>
+  </si>
+  <si>
+    <t>EnemyRatioUltimatesAll20_Control_Received_2 | EnemyRatioUltimatesAll20_Control_Received_1</t>
   </si>
   <si>
     <t>EnemyRatioUltimatesAll20 x Control_Received</t>
@@ -359,19 +365,43 @@
     <t>EnemyRatioUltimatesAll20 x ScorePerSecond</t>
   </si>
   <si>
-    <t>TeamRatioREX50_First_Orb</t>
-  </si>
-  <si>
-    <t>TeamRatioREX50 x First_Orb</t>
-  </si>
-  <si>
-    <t>TeamRatioREX50_Ultimates</t>
-  </si>
-  <si>
-    <t>TeamRatioREX50 x Ultimates</t>
-  </si>
-  <si>
-    <t>NetHealthShards_Control_Received_3 | NetHealthShards_Control_Received_1</t>
+    <t>TeamRatioREX50_NetOrbs</t>
+  </si>
+  <si>
+    <t>TeamRatioREX50 x NetOrbs</t>
+  </si>
+  <si>
+    <t>TeamRatioREX50_Ping</t>
+  </si>
+  <si>
+    <t>TeamRatioREX50 x Ping</t>
+  </si>
+  <si>
+    <t>EnemyRatioREX50_NetOrbs</t>
+  </si>
+  <si>
+    <t>EnemyRatioREX50 x NetOrbs</t>
+  </si>
+  <si>
+    <t>EnemyRatioREX50_Ultimates_2 | EnemyRatioREX50_Ultimates_3</t>
+  </si>
+  <si>
+    <t>EnemyRatioREX50 x Ultimates</t>
+  </si>
+  <si>
+    <t>NetHealthShards_NetOrbs</t>
+  </si>
+  <si>
+    <t>NetHealthShards x NetOrbs</t>
+  </si>
+  <si>
+    <t>NetHealthShards_Ultimates_2 | NetHealthShards_Ultimates_3</t>
+  </si>
+  <si>
+    <t>NetHealthShards x Ultimates</t>
+  </si>
+  <si>
+    <t>NetHealthShards_Control_Received_2 | NetHealthShards_Control_Received_1</t>
   </si>
   <si>
     <t>NetHealthShards x Control_Received</t>
@@ -383,43 +413,7 @@
     <t>NetHealthShards x Control</t>
   </si>
   <si>
-    <t>NetHealthShards_Protection</t>
-  </si>
-  <si>
-    <t>NetHealthShards x Protection</t>
-  </si>
-  <si>
-    <t>NetHealthShards_Damage_Received</t>
-  </si>
-  <si>
-    <t>NetHealthShards x Damage_Received</t>
-  </si>
-  <si>
-    <t>NetEnergyShards_3_Num_R</t>
-  </si>
-  <si>
-    <t>NetEnergyShards x Num_R</t>
-  </si>
-  <si>
-    <t>NetEnergyShards_3_Damage</t>
-  </si>
-  <si>
-    <t>NetEnergyShards x Damage</t>
-  </si>
-  <si>
-    <t>NetOrbs_EnemyRatioUltimatesAll20</t>
-  </si>
-  <si>
-    <t>NetOrbs x EnemyRatioUltimatesAll20</t>
-  </si>
-  <si>
-    <t>NetOrbs_EnemyRatioREX50</t>
-  </si>
-  <si>
-    <t>NetOrbs x EnemyRatioREX50</t>
-  </si>
-  <si>
-    <t>NetOrbs_Ultimates</t>
+    <t>NetOrbs_Ultimates_2 | NetOrbs_Ultimates_3</t>
   </si>
   <si>
     <t>NetOrbs x Ultimates</t>
@@ -431,46 +425,40 @@
     <t>NetOrbs x Num_R</t>
   </si>
   <si>
-    <t>NetOrbs_Control_Received_3 | NetOrbs_Control_Received_1</t>
+    <t>NetOrbs_Num_EX1_0.5 | NetOrbs_Num_EX1_1</t>
+  </si>
+  <si>
+    <t>NetOrbs x Num_EX1</t>
+  </si>
+  <si>
+    <t>NetOrbs_Num_EX2_3 | NetOrbs_Num_EX2_2</t>
+  </si>
+  <si>
+    <t>NetOrbs x Num_EX2</t>
+  </si>
+  <si>
+    <t>NetOrbs_Control_Received_2 | NetOrbs_Control_Received_1</t>
   </si>
   <si>
     <t>NetOrbs x Control_Received</t>
   </si>
   <si>
-    <t>NetOrbs_Control_0.5 | NetOrbs_Control_1</t>
-  </si>
-  <si>
-    <t>NetOrbs x Control</t>
-  </si>
-  <si>
-    <t>NetOrbs_Protection_Received</t>
-  </si>
-  <si>
-    <t>NetOrbs x Protection_Received</t>
-  </si>
-  <si>
     <t>NetOrbs_Protection</t>
   </si>
   <si>
     <t>NetOrbs x Protection</t>
   </si>
   <si>
-    <t>NetOrbs_Damage</t>
-  </si>
-  <si>
-    <t>NetOrbs x Damage</t>
-  </si>
-  <si>
-    <t>Ultimates_ScorePerSecond_1 | Ultimates_ScorePerSecond_2</t>
-  </si>
-  <si>
-    <t>Ultimates x ScorePerSecond</t>
-  </si>
-  <si>
-    <t>Num_R_TeamRatioREX50</t>
-  </si>
-  <si>
-    <t>Num_R x TeamRatioREX50</t>
+    <t>NetOrbs_Damage_Received</t>
+  </si>
+  <si>
+    <t>NetOrbs x Damage_Received</t>
+  </si>
+  <si>
+    <t>First_Orb_EnemyRatioREX50</t>
+  </si>
+  <si>
+    <t>First_Orb x EnemyRatioREX50</t>
   </si>
   <si>
     <t>Num_R_ScorePerSecond_1 | Num_R_ScorePerSecond_2</t>
@@ -479,58 +467,40 @@
     <t>Num_R x ScorePerSecond</t>
   </si>
   <si>
-    <t>Num_EX1_0.5_ScorePerSecond_1 | Num_EX1_0.5_ScorePerSecond_2 | Num_EX1_1_ScorePerSecond_1 | Num_EX1_1_ScorePerSecond_2</t>
-  </si>
-  <si>
-    <t>Num_EX1 x ScorePerSecond</t>
-  </si>
-  <si>
-    <t>Num_EX2_3_EnemyRatioUltimatesAll20 | Num_EX2_2_EnemyRatioUltimatesAll20</t>
-  </si>
-  <si>
-    <t>Num_EX2 x EnemyRatioUltimatesAll20</t>
-  </si>
-  <si>
-    <t>Num_EX2_3_NetOrbs | Num_EX2_2_NetOrbs</t>
-  </si>
-  <si>
-    <t>Num_EX2 x NetOrbs</t>
-  </si>
-  <si>
-    <t>Num_EX2_3_Ultimates | Num_EX2_2_Ultimates</t>
-  </si>
-  <si>
-    <t>Num_EX2 x Ultimates</t>
-  </si>
-  <si>
-    <t>Num_EX2_3_Num_R | Num_EX2_2_Num_R</t>
-  </si>
-  <si>
-    <t>Num_EX2 x Num_R</t>
-  </si>
-  <si>
-    <t>Num_EX2_3_ScorePerSecond_1 | Num_EX2_3_ScorePerSecond_2 | Num_EX2_2_ScorePerSecond_1 | Num_EX2_2_ScorePerSecond_2</t>
-  </si>
-  <si>
-    <t>Num_EX2 x ScorePerSecond</t>
-  </si>
-  <si>
-    <t>Control_Received_3_Protection | Control_Received_1_Protection</t>
-  </si>
-  <si>
-    <t>Control_Received x Protection</t>
-  </si>
-  <si>
-    <t>ScorePerSecond_1_TeamRatioUltimatesAll20 | ScorePerSecond_2_TeamRatioUltimatesAll20</t>
-  </si>
-  <si>
-    <t>ScorePerSecond x TeamRatioUltimatesAll20</t>
-  </si>
-  <si>
-    <t>ScorePerSecond_1_EnemyRatioREX50 | ScorePerSecond_2_EnemyRatioREX50</t>
-  </si>
-  <si>
-    <t>ScorePerSecond x EnemyRatioREX50</t>
+    <t>Damage_TeamRatioUltimatesAll20</t>
+  </si>
+  <si>
+    <t>Damage x TeamRatioUltimatesAll20</t>
+  </si>
+  <si>
+    <t>Damage_Protection</t>
+  </si>
+  <si>
+    <t>Damage x Protection</t>
+  </si>
+  <si>
+    <t>Ping_TeamRatioUltimatesAll20</t>
+  </si>
+  <si>
+    <t>Ping x TeamRatioUltimatesAll20</t>
+  </si>
+  <si>
+    <t>ScorePerSecond_1_Ultimates_2 | ScorePerSecond_1_Ultimates_3 | ScorePerSecond_2_Ultimates_2 | ScorePerSecond_2_Ultimates_3</t>
+  </si>
+  <si>
+    <t>ScorePerSecond x Ultimates</t>
+  </si>
+  <si>
+    <t>ScorePerSecond_1_Num_EX1_0.5 | ScorePerSecond_1_Num_EX1_1 | ScorePerSecond_2_Num_EX1_0.5 | ScorePerSecond_2_Num_EX1_1</t>
+  </si>
+  <si>
+    <t>ScorePerSecond x Num_EX1</t>
+  </si>
+  <si>
+    <t>ScorePerSecond_1_Num_EX2_3 | ScorePerSecond_1_Num_EX2_2 | ScorePerSecond_2_Num_EX2_3 | ScorePerSecond_2_Num_EX2_2</t>
+  </si>
+  <si>
+    <t>ScorePerSecond x Num_EX2</t>
   </si>
   <si>
     <t>Logistic Area Under Curve</t>
@@ -560,6 +530,12 @@
     <t>const</t>
   </si>
   <si>
+    <t>Ultimates_2</t>
+  </si>
+  <si>
+    <t>Ultimates_3</t>
+  </si>
+  <si>
     <t>Num_EX1_0.5</t>
   </si>
   <si>
@@ -572,7 +548,7 @@
     <t>Num_EX2_2</t>
   </si>
   <si>
-    <t>Control_Received_3</t>
+    <t>Control_Received_2</t>
   </si>
   <si>
     <t>Control_Received_1</t>
@@ -590,13 +566,31 @@
     <t>ScorePerSecond_2</t>
   </si>
   <si>
+    <t>TeamRatioUltimatesAll20_Ultimates_2</t>
+  </si>
+  <si>
+    <t>TeamRatioUltimatesAll20_Ultimates_3</t>
+  </si>
+  <si>
+    <t>TeamRatioUltimatesAll20_Num_EX1_0.5</t>
+  </si>
+  <si>
+    <t>TeamRatioUltimatesAll20_Num_EX1_1</t>
+  </si>
+  <si>
     <t>TeamRatioUltimatesAll20_Num_EX2_3</t>
   </si>
   <si>
     <t>TeamRatioUltimatesAll20_Num_EX2_2</t>
   </si>
   <si>
-    <t>EnemyRatioUltimatesAll20_Control_Received_3</t>
+    <t>EnemyRatioUltimatesAll20_Num_EX2_3</t>
+  </si>
+  <si>
+    <t>EnemyRatioUltimatesAll20_Num_EX2_2</t>
+  </si>
+  <si>
+    <t>EnemyRatioUltimatesAll20_Control_Received_2</t>
   </si>
   <si>
     <t>EnemyRatioUltimatesAll20_Control_Received_1</t>
@@ -608,7 +602,19 @@
     <t>EnemyRatioUltimatesAll20_ScorePerSecond_2</t>
   </si>
   <si>
-    <t>NetHealthShards_Control_Received_3</t>
+    <t>EnemyRatioREX50_Ultimates_2</t>
+  </si>
+  <si>
+    <t>EnemyRatioREX50_Ultimates_3</t>
+  </si>
+  <si>
+    <t>NetHealthShards_Ultimates_2</t>
+  </si>
+  <si>
+    <t>NetHealthShards_Ultimates_3</t>
+  </si>
+  <si>
+    <t>NetHealthShards_Control_Received_2</t>
   </si>
   <si>
     <t>NetHealthShards_Control_Received_1</t>
@@ -620,94 +626,70 @@
     <t>NetHealthShards_Control_1</t>
   </si>
   <si>
-    <t>NetOrbs_Control_Received_3</t>
+    <t>NetOrbs_Ultimates_2</t>
+  </si>
+  <si>
+    <t>NetOrbs_Ultimates_3</t>
+  </si>
+  <si>
+    <t>NetOrbs_Num_EX1_0.5</t>
+  </si>
+  <si>
+    <t>NetOrbs_Num_EX1_1</t>
+  </si>
+  <si>
+    <t>NetOrbs_Num_EX2_3</t>
+  </si>
+  <si>
+    <t>NetOrbs_Num_EX2_2</t>
+  </si>
+  <si>
+    <t>NetOrbs_Control_Received_2</t>
   </si>
   <si>
     <t>NetOrbs_Control_Received_1</t>
   </si>
   <si>
-    <t>NetOrbs_Control_0.5</t>
-  </si>
-  <si>
-    <t>NetOrbs_Control_1</t>
-  </si>
-  <si>
-    <t>Ultimates_ScorePerSecond_1</t>
-  </si>
-  <si>
-    <t>Ultimates_ScorePerSecond_2</t>
-  </si>
-  <si>
     <t>Num_R_ScorePerSecond_1</t>
   </si>
   <si>
     <t>Num_R_ScorePerSecond_2</t>
   </si>
   <si>
-    <t>Num_EX1_0.5_ScorePerSecond_1</t>
-  </si>
-  <si>
-    <t>Num_EX1_0.5_ScorePerSecond_2</t>
-  </si>
-  <si>
-    <t>Num_EX1_1_ScorePerSecond_1</t>
-  </si>
-  <si>
-    <t>Num_EX1_1_ScorePerSecond_2</t>
-  </si>
-  <si>
-    <t>Num_EX2_3_EnemyRatioUltimatesAll20</t>
-  </si>
-  <si>
-    <t>Num_EX2_2_EnemyRatioUltimatesAll20</t>
-  </si>
-  <si>
-    <t>Num_EX2_3_NetOrbs</t>
-  </si>
-  <si>
-    <t>Num_EX2_2_NetOrbs</t>
-  </si>
-  <si>
-    <t>Num_EX2_3_Ultimates</t>
-  </si>
-  <si>
-    <t>Num_EX2_2_Ultimates</t>
-  </si>
-  <si>
-    <t>Num_EX2_3_Num_R</t>
-  </si>
-  <si>
-    <t>Num_EX2_2_Num_R</t>
-  </si>
-  <si>
-    <t>Num_EX2_3_ScorePerSecond_1</t>
-  </si>
-  <si>
-    <t>Num_EX2_3_ScorePerSecond_2</t>
-  </si>
-  <si>
-    <t>Num_EX2_2_ScorePerSecond_1</t>
-  </si>
-  <si>
-    <t>Num_EX2_2_ScorePerSecond_2</t>
-  </si>
-  <si>
-    <t>Control_Received_3_Protection</t>
-  </si>
-  <si>
-    <t>Control_Received_1_Protection</t>
-  </si>
-  <si>
-    <t>ScorePerSecond_1_TeamRatioUltimatesAll20</t>
-  </si>
-  <si>
-    <t>ScorePerSecond_2_TeamRatioUltimatesAll20</t>
-  </si>
-  <si>
-    <t>ScorePerSecond_1_EnemyRatioREX50</t>
-  </si>
-  <si>
-    <t>ScorePerSecond_2_EnemyRatioREX50</t>
+    <t>ScorePerSecond_1_Ultimates_2</t>
+  </si>
+  <si>
+    <t>ScorePerSecond_1_Ultimates_3</t>
+  </si>
+  <si>
+    <t>ScorePerSecond_2_Ultimates_2</t>
+  </si>
+  <si>
+    <t>ScorePerSecond_2_Ultimates_3</t>
+  </si>
+  <si>
+    <t>ScorePerSecond_1_Num_EX1_0.5</t>
+  </si>
+  <si>
+    <t>ScorePerSecond_1_Num_EX1_1</t>
+  </si>
+  <si>
+    <t>ScorePerSecond_2_Num_EX1_0.5</t>
+  </si>
+  <si>
+    <t>ScorePerSecond_2_Num_EX1_1</t>
+  </si>
+  <si>
+    <t>ScorePerSecond_1_Num_EX2_3</t>
+  </si>
+  <si>
+    <t>ScorePerSecond_1_Num_EX2_2</t>
+  </si>
+  <si>
+    <t>ScorePerSecond_2_Num_EX2_3</t>
+  </si>
+  <si>
+    <t>ScorePerSecond_2_Num_EX2_2</t>
   </si>
 </sst>
 </file>
@@ -1235,10 +1217,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>58692</v>
+        <v>58512</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>7</v>
@@ -1250,12 +1232,12 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>74094</v>
+        <v>73991</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="n">
         <v>58512</v>
@@ -1270,7 +1252,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>30017</v>
+        <v>29976</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1287,7 +1269,7 @@
         <v>2</v>
       </c>
       <c r="H6" t="n">
-        <v>9963</v>
+        <v>9937</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1295,7 +1277,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>66870</v>
+        <v>66782</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
@@ -1307,7 +1289,7 @@
         <v>3</v>
       </c>
       <c r="H7" t="n">
-        <v>2498</v>
+        <v>2492</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1315,7 +1297,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>50334</v>
+        <v>50242</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>12</v>
@@ -1327,7 +1309,7 @@
         <v>4</v>
       </c>
       <c r="H8" t="n">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1341,7 +1323,7 @@
         <v>5</v>
       </c>
       <c r="H9" t="n">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1349,7 +1331,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>66870</v>
+        <v>66782</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>7</v>
@@ -1369,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="n">
-        <v>50334</v>
+        <v>50242</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>8</v>
@@ -1406,7 +1388,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="n">
-        <v>87250</v>
+        <v>87118</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>11</v>
@@ -1420,7 +1402,7 @@
         <v>0</v>
       </c>
       <c r="B14" t="n">
-        <v>29954</v>
+        <v>29906</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>12</v>
@@ -1442,7 +1424,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="n">
-        <v>87250</v>
+        <v>87118</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>7</v>
@@ -1456,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="n">
-        <v>29954</v>
+        <v>29906</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>8</v>
@@ -1481,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="B19" t="n">
-        <v>62528</v>
+        <v>62436</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>11</v>
@@ -1495,7 +1477,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="n">
-        <v>54676</v>
+        <v>54588</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>12</v>
@@ -1792,7 +1774,7 @@
         <v>8</v>
       </c>
       <c r="E59" t="n">
-        <v>39.4</v>
+        <v>39.249076</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2017,7 +1999,7 @@
         <v>8</v>
       </c>
       <c r="E89" t="n">
-        <v>2.604651162790698</v>
+        <v>2.702381563239237</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2025,7 +2007,7 @@
         <v>10</v>
       </c>
       <c r="E90" t="n">
-        <v>5.228076948184414</v>
+        <v>5.343522463018814</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2033,7 +2015,7 @@
         <v>11</v>
       </c>
       <c r="E91" t="n">
-        <v>7.674418604651162</v>
+        <v>7.813879938358083</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2041,7 +2023,7 @@
         <v>12</v>
       </c>
       <c r="E92" t="n">
-        <v>61.70874</v>
+        <v>85.65263684210524</v>
       </c>
     </row>
   </sheetData>
@@ -2071,49 +2053,49 @@
   <sheetData>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B16" t="n">
-        <v>0.9543829276770652</v>
+        <v>0.9531773391068323</v>
       </c>
       <c r="F16" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="G16" t="n">
-        <v>0.9675218255124843</v>
+        <v>0.9666607509422596</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B17" t="n">
         <v>0.5</v>
       </c>
       <c r="F17" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G17" t="n">
-        <v>0.9095987404488485</v>
+        <v>0.9077250913258362</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B18" t="n">
-        <v>0.5932262261053417</v>
+        <v>0.5853368517567632</v>
       </c>
       <c r="F18" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="G18" t="n">
-        <v>0.7496160540595884</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="F19" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
@@ -2121,10 +2103,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="F20" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G20" t="n">
-        <v>0.5200000000000002</v>
+        <v>0.5500000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -2139,7 +2121,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:B85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2153,18 +2135,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B2" t="n">
-        <v>4.21446117989697</v>
+        <v>4.340568395744372</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2172,7 +2154,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6337897548281377</v>
+        <v>1.195403695994451</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2180,7 +2162,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="n">
-        <v>0.149239785824363</v>
+        <v>-0.1359147003759697</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2188,7 +2170,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.05048502589891985</v>
+        <v>-0.2540899777586974</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2196,7 +2178,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2131846943309656</v>
+        <v>0.266458653405292</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2204,7 +2186,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1169669015647042</v>
+        <v>0.0783047978762272</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2212,7 +2194,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>1.121791595395281</v>
+        <v>0.9482380638705185</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2220,407 +2202,407 @@
         <v>18</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.7515921079724296</v>
+        <v>-0.7132292944872535</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B10" t="n">
-        <v>1.679353729266305</v>
+        <v>0.7539839168574478</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B11" t="n">
-        <v>0.8621316621333579</v>
+        <v>0.01784998754049509</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" t="n">
-        <v>0.01876474019350841</v>
+        <v>0.009396415108266708</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" t="n">
-        <v>0.007408657501849077</v>
+        <v>-0.02178174483079786</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.02301067871429597</v>
+        <v>0.007959484786784212</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" t="n">
-        <v>0.005493395761945968</v>
+        <v>4.959505578296599e-10</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="B16" t="n">
-        <v>-5.272518389064298e-05</v>
+        <v>0.3969841334594242</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B17" t="n">
-        <v>0.9530303594546186</v>
+        <v>-0.03381213301532577</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B18" t="n">
-        <v>0.3376926349472214</v>
+        <v>1.228850594980529</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B19" t="n">
-        <v>0.01165970495740261</v>
+        <v>0.01917419883632759</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B20" t="n">
-        <v>0.02507975082603667</v>
+        <v>0.006434872040430317</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B21" t="n">
-        <v>1.224632089369337e-07</v>
+        <v>0.01406730448916377</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.007282678231026981</v>
+        <v>3.601786600128678e-05</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B23" t="n">
-        <v>0.3159014240666357</v>
+        <v>-0.01329649329754483</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.01723984339667391</v>
+        <v>0.2817407888120395</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>177</v>
       </c>
       <c r="B25" t="n">
-        <v>2.516666195577591</v>
+        <v>-0.01555849689270198</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B26" t="n">
-        <v>-0.7040898764073198</v>
+        <v>-0.875979131058263</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B27" t="n">
-        <v>0.03314526838946755</v>
+        <v>0.04487476959798088</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B28" t="n">
-        <v>0.05455456336343179</v>
+        <v>0.03580483691239531</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B29" t="n">
-        <v>0.1440819515575036</v>
+        <v>-0.0004496155819608852</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.554824706992383</v>
+        <v>-0.01844246330406791</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>180</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.06259404214621517</v>
+        <v>-0.1221257972902583</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B32" t="n">
-        <v>-0.002679731381121991</v>
+        <v>0.008603324349815235</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>189</v>
+        <v>99</v>
       </c>
       <c r="B33" t="n">
-        <v>0.01668661358562649</v>
+        <v>0.02508404566472359</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>182</v>
       </c>
       <c r="B34" t="n">
-        <v>-0.1312838190128848</v>
+        <v>0.06881438917758698</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B35" t="n">
-        <v>-2.046530211926264e-08</v>
+        <v>0.0244546598302969</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B36" t="n">
-        <v>0.004265604964130813</v>
+        <v>0.003958427451230585</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.06488525717820047</v>
+        <v>-0.03118195877712828</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>193</v>
+        <v>105</v>
       </c>
       <c r="B38" t="n">
-        <v>0.005874924120490921</v>
+        <v>-0.0008560283533267565</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>186</v>
       </c>
       <c r="B39" t="n">
-        <v>0.02852492348331729</v>
+        <v>-0.001457699202703184</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>113</v>
+        <v>187</v>
       </c>
       <c r="B40" t="n">
-        <v>-0.04213939554503138</v>
+        <v>0.03135909060208533</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B41" t="n">
-        <v>2.547472882107318e-09</v>
+        <v>-9.944578390081296e-06</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B42" t="n">
-        <v>-0.0003596392650739528</v>
+        <v>0.005601021420605934</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B43" t="n">
-        <v>0.004105603075613654</v>
+        <v>-0.03357103357993284</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B44" t="n">
-        <v>-0.0002884209031781609</v>
+        <v>0.004533552537536528</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B45" t="n">
-        <v>0.0001605116154109385</v>
+        <v>0.03176325492890845</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B46" t="n">
-        <v>-0.0002220413174312878</v>
+        <v>1.209301627905258e-09</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B47" t="n">
-        <v>0.0001081733084115</v>
+        <v>0.06182995184093774</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>125</v>
+        <v>192</v>
       </c>
       <c r="B48" t="n">
-        <v>-6.647573874090089e-08</v>
+        <v>-0.002321079351711493</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>127</v>
+        <v>193</v>
       </c>
       <c r="B49" t="n">
-        <v>-0.01953202343118419</v>
+        <v>-0.0006405590576891233</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B50" t="n">
-        <v>0.03856568422862778</v>
+        <v>-0.003770747128520466</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="B51" t="n">
-        <v>0.0411777003696859</v>
+        <v>0.002978882893880173</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>133</v>
+        <v>195</v>
       </c>
       <c r="B52" t="n">
-        <v>0.01069248678277657</v>
+        <v>-0.001450513254617879</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B53" t="n">
-        <v>1.440431307730017e-08</v>
+        <v>1.128296994262365e-06</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B54" t="n">
-        <v>-0.001687210974597861</v>
+        <v>-0.0006158622252648564</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B55" t="n">
-        <v>-0.0395269203981253</v>
+        <v>0.003611035235091764</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B56" t="n">
-        <v>0.001943011676308447</v>
+        <v>-0.0003582257242115585</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>139</v>
+        <v>200</v>
       </c>
       <c r="B57" t="n">
-        <v>-0.0001626643430687497</v>
+        <v>-0.0128884974243642</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>141</v>
+        <v>201</v>
       </c>
       <c r="B58" t="n">
-        <v>-5.414938839653097e-05</v>
+        <v>0.001312285829782322</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="B59" t="n">
-        <v>-0.0005894414853187071</v>
+        <v>-0.009092743150023116</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -2628,7 +2610,7 @@
         <v>202</v>
       </c>
       <c r="B60" t="n">
-        <v>-0.3026380710436554</v>
+        <v>-0.02982217605454475</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -2636,207 +2618,199 @@
         <v>203</v>
       </c>
       <c r="B61" t="n">
-        <v>0.01313275712373569</v>
+        <v>0.0005914648786580954</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>147</v>
+        <v>204</v>
       </c>
       <c r="B62" t="n">
-        <v>-0.1657324618567219</v>
+        <v>-0.0001473939751615185</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B63" t="n">
-        <v>-0.1544462642694883</v>
+        <v>-0.005145811477953868</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B64" t="n">
-        <v>0.007597973579039329</v>
+        <v>5.685097863156076e-06</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B65" t="n">
-        <v>-0.2111139041840708</v>
+        <v>-0.002222204292608859</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>207</v>
+        <v>139</v>
       </c>
       <c r="B66" t="n">
-        <v>0.01369937590981683</v>
+        <v>0.0001867671974344502</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>208</v>
+        <v>141</v>
       </c>
       <c r="B67" t="n">
-        <v>-0.07791158926675279</v>
+        <v>-0.0006663169634479146</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>209</v>
+        <v>143</v>
       </c>
       <c r="B68" t="n">
-        <v>0.002587999473344602</v>
+        <v>0.03929164655918029</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B69" t="n">
-        <v>-0.001526207336580435</v>
+        <v>-0.1736057171451098</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B70" t="n">
-        <v>0.03547632049568534</v>
+        <v>0.009023346520482711</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>212</v>
+        <v>147</v>
       </c>
       <c r="B71" t="n">
-        <v>-0.0008514638848867727</v>
+        <v>-0.001742670155020872</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>213</v>
+        <v>149</v>
       </c>
       <c r="B72" t="n">
-        <v>0.001765770761386781</v>
+        <v>-1.017988513180691e-05</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>214</v>
+        <v>151</v>
       </c>
       <c r="B73" t="n">
-        <v>0.005274909911126262</v>
+        <v>-1.061415048651598e-09</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B74" t="n">
-        <v>-0.04905512171735366</v>
+        <v>-0.07427481635682487</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B75" t="n">
-        <v>-0.0009035524336244845</v>
+        <v>0.007254309219867428</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B76" t="n">
-        <v>0.008448428430306281</v>
+        <v>0.001848212642937167</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B77" t="n">
-        <v>-0.001352347099719389</v>
+        <v>7.142893438473536e-05</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B78" t="n">
-        <v>8.439104023818155e-05</v>
+        <v>-0.2565147994930377</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B79" t="n">
-        <v>-0.01752343890866684</v>
+        <v>-0.004139299291523904</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B80" t="n">
-        <v>0.0007080064710305915</v>
+        <v>0.01371157001369507</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B81" t="n">
-        <v>7.190948966591521e-11</v>
+        <v>-0.0006050975852673757</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B82" t="n">
-        <v>-2.503665438208296e-05</v>
+        <v>-0.001586135377555645</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B83" t="n">
-        <v>-0.08187849574570846</v>
+        <v>-0.00368421913275097</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B84" t="n">
-        <v>0.008005385879980358</v>
+        <v>0.0001463471880203925</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B85" t="n">
-        <v>0.02219787348030473</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" t="s">
-        <v>227</v>
-      </c>
-      <c r="B86" t="n">
-        <v>-0.0010864907811205</v>
+        <v>-0.0003902789463585724</v>
       </c>
     </row>
   </sheetData>
@@ -2850,7 +2824,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2882,7 +2856,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="6" t="n">
-        <v>7.424124870956083e-96</v>
+        <v>8.50543894920259e-97</v>
       </c>
       <c r="C2" s="6" t="n"/>
       <c r="D2" s="6" t="n"/>
@@ -2897,7 +2871,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="6" t="n">
-        <v>1.952203327155908e-97</v>
+        <v>8.505438949078495e-97</v>
       </c>
       <c r="C3" s="6" t="n"/>
       <c r="D3" s="6" t="n"/>
@@ -2912,7 +2886,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="6" t="n">
-        <v>8.036732892823037e-174</v>
+        <v>2.828570726796667e-174</v>
       </c>
       <c r="C4" s="6" t="n"/>
       <c r="D4" s="6" t="n"/>
@@ -2927,7 +2901,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="6" t="n">
-        <v>3.499656814284619e-174</v>
+        <v>2.828570718389073e-174</v>
       </c>
       <c r="C5" s="6" t="n"/>
       <c r="D5" s="6" t="n"/>
@@ -2942,7 +2916,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="n">
-        <v>3.573445816697813e-304</v>
+        <v>7.594216200611275e-305</v>
       </c>
       <c r="C6" s="6" t="n"/>
       <c r="D6" s="6" t="n"/>
@@ -2957,7 +2931,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="6" t="n">
-        <v>2.161648322653635e-95</v>
+        <v>1.412777504189132e-95</v>
       </c>
       <c r="C7" s="6" t="n"/>
       <c r="D7" s="6" t="n"/>
@@ -3002,7 +2976,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="6" t="n">
-        <v>2.197142580512923e-209</v>
+        <v>7.76924209348726e-212</v>
       </c>
       <c r="C10" s="6" t="n"/>
       <c r="D10" s="6" t="n"/>
@@ -3017,7 +2991,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="6" t="n">
-        <v>1.010946826006109e-135</v>
+        <v>2.071673189789999e-137</v>
       </c>
       <c r="C11" s="6" t="n"/>
       <c r="D11" s="6" t="n"/>
@@ -3032,7 +3006,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="6" t="n">
-        <v>1.407383825038449e-286</v>
+        <v>4.140584509349334e-288</v>
       </c>
       <c r="C12" s="6" t="n"/>
       <c r="D12" s="6" t="n"/>
@@ -3047,7 +3021,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="6" t="n">
-        <v>8.495795672388451e-253</v>
+        <v>4.151999017444018e-254</v>
       </c>
       <c r="C13" s="6" t="n"/>
       <c r="D13" s="6" t="n"/>
@@ -3092,7 +3066,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="6" t="n">
-        <v>3.381784429358499e-305</v>
+        <v>3.399410879357983e-309</v>
       </c>
       <c r="C16" s="6" t="n"/>
       <c r="D16" s="6" t="n"/>
@@ -3107,7 +3081,7 @@
         <v>25</v>
       </c>
       <c r="B17" s="6" t="n">
-        <v>1.796524453153868e-128</v>
+        <v>9.212436836243791e-130</v>
       </c>
       <c r="C17" s="6" t="n"/>
       <c r="D17" s="6" t="n"/>
@@ -3152,7 +3126,7 @@
         <v>28</v>
       </c>
       <c r="B20" s="6" t="n">
-        <v>0.0003326627967452281</v>
+        <v>0.0003466456876842633</v>
       </c>
       <c r="C20" s="6" t="n"/>
       <c r="D20" s="6" t="n"/>
@@ -3418,39 +3392,6 @@
       <c r="G43" s="6" t="n"/>
       <c r="H43" s="6" t="n"/>
       <c r="I43" s="6" t="n"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="6" t="n"/>
-      <c r="B44" s="6" t="n"/>
-      <c r="C44" s="6" t="n"/>
-      <c r="D44" s="6" t="n"/>
-      <c r="E44" s="6" t="n"/>
-      <c r="F44" s="6" t="n"/>
-      <c r="G44" s="6" t="n"/>
-      <c r="H44" s="6" t="n"/>
-      <c r="I44" s="6" t="n"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="6" t="n"/>
-      <c r="B45" s="6" t="n"/>
-      <c r="C45" s="6" t="n"/>
-      <c r="D45" s="6" t="n"/>
-      <c r="E45" s="6" t="n"/>
-      <c r="F45" s="6" t="n"/>
-      <c r="G45" s="6" t="n"/>
-      <c r="H45" s="6" t="n"/>
-      <c r="I45" s="6" t="n"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="6" t="n"/>
-      <c r="B46" s="6" t="n"/>
-      <c r="C46" s="6" t="n"/>
-      <c r="D46" s="6" t="n"/>
-      <c r="E46" s="6" t="n"/>
-      <c r="F46" s="6" t="n"/>
-      <c r="G46" s="6" t="n"/>
-      <c r="H46" s="6" t="n"/>
-      <c r="I46" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -3463,7 +3404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3952,39 +3893,6 @@
       <c r="H43" s="6" t="n"/>
       <c r="I43" s="6" t="n"/>
     </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="6" t="n"/>
-      <c r="B44" s="6" t="n"/>
-      <c r="C44" s="6" t="n"/>
-      <c r="D44" s="6" t="n"/>
-      <c r="E44" s="6" t="n"/>
-      <c r="F44" s="6" t="n"/>
-      <c r="G44" s="6" t="n"/>
-      <c r="H44" s="6" t="n"/>
-      <c r="I44" s="6" t="n"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="6" t="n"/>
-      <c r="B45" s="6" t="n"/>
-      <c r="C45" s="6" t="n"/>
-      <c r="D45" s="6" t="n"/>
-      <c r="E45" s="6" t="n"/>
-      <c r="F45" s="6" t="n"/>
-      <c r="G45" s="6" t="n"/>
-      <c r="H45" s="6" t="n"/>
-      <c r="I45" s="6" t="n"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="6" t="n"/>
-      <c r="B46" s="6" t="n"/>
-      <c r="C46" s="6" t="n"/>
-      <c r="D46" s="6" t="n"/>
-      <c r="E46" s="6" t="n"/>
-      <c r="F46" s="6" t="n"/>
-      <c r="G46" s="6" t="n"/>
-      <c r="H46" s="6" t="n"/>
-      <c r="I46" s="6" t="n"/>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -3996,7 +3904,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4148,10 +4056,10 @@
         <v>40</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F7" s="6" t="n"/>
       <c r="G7" s="6" t="n"/>
@@ -4693,39 +4601,6 @@
       <c r="G43" s="6" t="n"/>
       <c r="H43" s="6" t="n"/>
       <c r="I43" s="6" t="n"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="6" t="n"/>
-      <c r="B44" s="6" t="n"/>
-      <c r="C44" s="6" t="n"/>
-      <c r="D44" s="6" t="n"/>
-      <c r="E44" s="6" t="n"/>
-      <c r="F44" s="6" t="n"/>
-      <c r="G44" s="6" t="n"/>
-      <c r="H44" s="6" t="n"/>
-      <c r="I44" s="6" t="n"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="6" t="n"/>
-      <c r="B45" s="6" t="n"/>
-      <c r="C45" s="6" t="n"/>
-      <c r="D45" s="6" t="n"/>
-      <c r="E45" s="6" t="n"/>
-      <c r="F45" s="6" t="n"/>
-      <c r="G45" s="6" t="n"/>
-      <c r="H45" s="6" t="n"/>
-      <c r="I45" s="6" t="n"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="6" t="n"/>
-      <c r="B46" s="6" t="n"/>
-      <c r="C46" s="6" t="n"/>
-      <c r="D46" s="6" t="n"/>
-      <c r="E46" s="6" t="n"/>
-      <c r="F46" s="6" t="n"/>
-      <c r="G46" s="6" t="n"/>
-      <c r="H46" s="6" t="n"/>
-      <c r="I46" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -4738,7 +4613,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5236,39 +5111,6 @@
       <c r="H43" s="6" t="n"/>
       <c r="I43" s="6" t="n"/>
     </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="6" t="n"/>
-      <c r="B44" s="6" t="n"/>
-      <c r="C44" s="6" t="n"/>
-      <c r="D44" s="6" t="n"/>
-      <c r="E44" s="6" t="n"/>
-      <c r="F44" s="6" t="n"/>
-      <c r="G44" s="6" t="n"/>
-      <c r="H44" s="6" t="n"/>
-      <c r="I44" s="6" t="n"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="6" t="n"/>
-      <c r="B45" s="6" t="n"/>
-      <c r="C45" s="6" t="n"/>
-      <c r="D45" s="6" t="n"/>
-      <c r="E45" s="6" t="n"/>
-      <c r="F45" s="6" t="n"/>
-      <c r="G45" s="6" t="n"/>
-      <c r="H45" s="6" t="n"/>
-      <c r="I45" s="6" t="n"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="6" t="n"/>
-      <c r="B46" s="6" t="n"/>
-      <c r="C46" s="6" t="n"/>
-      <c r="D46" s="6" t="n"/>
-      <c r="E46" s="6" t="n"/>
-      <c r="F46" s="6" t="n"/>
-      <c r="G46" s="6" t="n"/>
-      <c r="H46" s="6" t="n"/>
-      <c r="I46" s="6" t="n"/>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -5280,7 +5122,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5397,7 +5239,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>40</v>
@@ -5414,13 +5256,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D8" s="6" t="n"/>
       <c r="E8" s="6" t="n"/>
@@ -5431,13 +5273,13 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="6" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D9" s="6" t="n"/>
       <c r="E9" s="6" t="n"/>
@@ -5448,7 +5290,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="6" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>40</v>
@@ -5465,7 +5307,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>40</v>
@@ -5482,7 +5324,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>40</v>
@@ -5499,7 +5341,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>40</v>
@@ -5516,7 +5358,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>40</v>
@@ -5533,7 +5375,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>40</v>
@@ -5550,7 +5392,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>40</v>
@@ -5567,7 +5409,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>40</v>
@@ -5584,7 +5426,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>40</v>
@@ -5601,7 +5443,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>40</v>
@@ -5618,7 +5460,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>40</v>
@@ -5634,15 +5476,9 @@
       <c r="I20" s="6" t="n"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="A21" s="6" t="n"/>
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="6" t="n"/>
       <c r="D21" s="6" t="n"/>
       <c r="E21" s="6" t="n"/>
       <c r="F21" s="6" t="n"/>
@@ -5891,39 +5727,6 @@
       <c r="G43" s="6" t="n"/>
       <c r="H43" s="6" t="n"/>
       <c r="I43" s="6" t="n"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="6" t="n"/>
-      <c r="B44" s="6" t="n"/>
-      <c r="C44" s="6" t="n"/>
-      <c r="D44" s="6" t="n"/>
-      <c r="E44" s="6" t="n"/>
-      <c r="F44" s="6" t="n"/>
-      <c r="G44" s="6" t="n"/>
-      <c r="H44" s="6" t="n"/>
-      <c r="I44" s="6" t="n"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="6" t="n"/>
-      <c r="B45" s="6" t="n"/>
-      <c r="C45" s="6" t="n"/>
-      <c r="D45" s="6" t="n"/>
-      <c r="E45" s="6" t="n"/>
-      <c r="F45" s="6" t="n"/>
-      <c r="G45" s="6" t="n"/>
-      <c r="H45" s="6" t="n"/>
-      <c r="I45" s="6" t="n"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="6" t="n"/>
-      <c r="B46" s="6" t="n"/>
-      <c r="C46" s="6" t="n"/>
-      <c r="D46" s="6" t="n"/>
-      <c r="E46" s="6" t="n"/>
-      <c r="F46" s="6" t="n"/>
-      <c r="G46" s="6" t="n"/>
-      <c r="H46" s="6" t="n"/>
-      <c r="I46" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -5936,7 +5739,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5957,19 +5760,19 @@
         <v>30</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G1" s="6" t="n"/>
       <c r="H1" s="6" t="n"/>
@@ -5980,13 +5783,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>40</v>
@@ -6003,19 +5806,19 @@
         <v>5</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C3" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G3" s="6" t="n"/>
       <c r="H3" s="6" t="n"/>
@@ -6026,7 +5829,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C4" s="6" t="n">
         <v>4</v>
@@ -6046,16 +5849,16 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>40</v>
@@ -6069,22 +5872,22 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C6" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G6" s="6" t="n"/>
       <c r="H6" s="6" t="n"/>
@@ -6092,22 +5895,22 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C7" s="6" t="n">
         <v>4</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="G7" s="6" t="n"/>
       <c r="H7" s="6" t="n"/>
@@ -6115,16 +5918,16 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C8" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>40</v>
@@ -6138,19 +5941,19 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C9" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>58</v>
@@ -6161,22 +5964,22 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C10" s="6" t="n">
         <v>4</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="G10" s="6" t="n"/>
       <c r="H10" s="6" t="n"/>
@@ -6184,16 +5987,16 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="6" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C11" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>40</v>
@@ -6207,22 +6010,22 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="6" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C12" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="G12" s="6" t="n"/>
       <c r="H12" s="6" t="n"/>
@@ -6230,10 +6033,10 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="6" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C13" s="6" t="n">
         <v>4</v>
@@ -6253,16 +6056,16 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C14" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>40</v>
@@ -6276,22 +6079,22 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C15" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G15" s="6" t="n"/>
       <c r="H15" s="6" t="n"/>
@@ -6299,22 +6102,22 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C16" s="6" t="n">
         <v>4</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="G16" s="6" t="n"/>
       <c r="H16" s="6" t="n"/>
@@ -6322,16 +6125,16 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C17" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>40</v>
@@ -6345,22 +6148,22 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C18" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G18" s="6" t="n"/>
       <c r="H18" s="6" t="n"/>
@@ -6368,22 +6171,22 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C19" s="6" t="n">
         <v>4</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G19" s="6" t="n"/>
       <c r="H19" s="6" t="n"/>
@@ -6391,16 +6194,16 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C20" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>40</v>
@@ -6414,22 +6217,22 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C21" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G21" s="6" t="n"/>
       <c r="H21" s="6" t="n"/>
@@ -6437,22 +6240,22 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C22" s="6" t="n">
         <v>4</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G22" s="6" t="n"/>
       <c r="H22" s="6" t="n"/>
@@ -6460,16 +6263,16 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C23" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>40</v>
@@ -6483,22 +6286,22 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C24" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G24" s="6" t="n"/>
       <c r="H24" s="6" t="n"/>
@@ -6506,10 +6309,10 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C25" s="6" t="n">
         <v>4</v>
@@ -6518,10 +6321,10 @@
         <v>72</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G25" s="6" t="n"/>
       <c r="H25" s="6" t="n"/>
@@ -6529,16 +6332,16 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C26" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>40</v>
@@ -6552,10 +6355,10 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C27" s="6" t="n">
         <v>2</v>
@@ -6564,7 +6367,7 @@
         <v>73</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>58</v>
@@ -6575,22 +6378,22 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C28" s="6" t="n">
         <v>4</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="G28" s="6" t="n"/>
       <c r="H28" s="6" t="n"/>
@@ -6598,16 +6401,16 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C29" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>40</v>
@@ -6621,22 +6424,22 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C30" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G30" s="6" t="n"/>
       <c r="H30" s="6" t="n"/>
@@ -6644,10 +6447,10 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C31" s="6" t="n">
         <v>4</v>
@@ -6667,16 +6470,16 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C32" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>40</v>
@@ -6690,22 +6493,22 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C33" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G33" s="6" t="n"/>
       <c r="H33" s="6" t="n"/>
@@ -6713,10 +6516,10 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C34" s="6" t="n">
         <v>4</v>
@@ -6736,16 +6539,16 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C35" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>40</v>
@@ -6759,22 +6562,22 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C36" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G36" s="6" t="n"/>
       <c r="H36" s="6" t="n"/>
@@ -6782,10 +6585,10 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C37" s="6" t="n">
         <v>4</v>
@@ -6805,16 +6608,16 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C38" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>40</v>
@@ -6828,19 +6631,19 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C39" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>78</v>
@@ -6851,10 +6654,10 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C40" s="6" t="n">
         <v>4</v>
@@ -6874,16 +6677,16 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C41" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>40</v>
@@ -6897,10 +6700,10 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C42" s="6" t="n">
         <v>2</v>
@@ -6909,10 +6712,10 @@
         <v>79</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G42" s="6" t="n"/>
       <c r="H42" s="6" t="n"/>
@@ -6920,10 +6723,10 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C43" s="6" t="n">
         <v>4</v>
@@ -6932,7 +6735,7 @@
         <v>80</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>81</v>
@@ -6940,75 +6743,6 @@
       <c r="G43" s="6" t="n"/>
       <c r="H43" s="6" t="n"/>
       <c r="I43" s="6" t="n"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G44" s="6" t="n"/>
-      <c r="H44" s="6" t="n"/>
-      <c r="I44" s="6" t="n"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G45" s="6" t="n"/>
-      <c r="H45" s="6" t="n"/>
-      <c r="I45" s="6" t="n"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G46" s="6" t="n"/>
-      <c r="H46" s="6" t="n"/>
-      <c r="I46" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -7021,7 +6755,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7038,7 +6772,7 @@
         <v>30</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C1" s="6" t="n"/>
       <c r="D1" s="6" t="n"/>
@@ -7065,10 +6799,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C3" s="6" t="n"/>
       <c r="D3" s="6" t="n"/>
@@ -7080,10 +6814,10 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="C4" s="6" t="n"/>
       <c r="D4" s="6" t="n"/>
@@ -7095,7 +6829,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="6" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>40</v>
@@ -7110,10 +6844,10 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="C6" s="6" t="n"/>
       <c r="D6" s="6" t="n"/>
@@ -7125,10 +6859,10 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C7" s="6" t="n"/>
       <c r="D7" s="6" t="n"/>
@@ -7140,10 +6874,10 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C8" s="6" t="n"/>
       <c r="D8" s="6" t="n"/>
@@ -7155,10 +6889,10 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C9" s="6" t="n"/>
       <c r="D9" s="6" t="n"/>
@@ -7170,10 +6904,10 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="C10" s="6" t="n"/>
       <c r="D10" s="6" t="n"/>
@@ -7185,7 +6919,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>40</v>
@@ -7200,7 +6934,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>40</v>
@@ -7215,7 +6949,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>40</v>
@@ -7230,7 +6964,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>40</v>
@@ -7245,10 +6979,10 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C15" s="6" t="n"/>
       <c r="D15" s="6" t="n"/>
@@ -7259,12 +6993,8 @@
       <c r="I15" s="6" t="n"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="A16" s="6" t="n"/>
+      <c r="B16" s="6" t="n"/>
       <c r="C16" s="6" t="n"/>
       <c r="D16" s="6" t="n"/>
       <c r="E16" s="6" t="n"/>
@@ -7569,39 +7299,6 @@
       <c r="G43" s="6" t="n"/>
       <c r="H43" s="6" t="n"/>
       <c r="I43" s="6" t="n"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="6" t="n"/>
-      <c r="B44" s="6" t="n"/>
-      <c r="C44" s="6" t="n"/>
-      <c r="D44" s="6" t="n"/>
-      <c r="E44" s="6" t="n"/>
-      <c r="F44" s="6" t="n"/>
-      <c r="G44" s="6" t="n"/>
-      <c r="H44" s="6" t="n"/>
-      <c r="I44" s="6" t="n"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="6" t="n"/>
-      <c r="B45" s="6" t="n"/>
-      <c r="C45" s="6" t="n"/>
-      <c r="D45" s="6" t="n"/>
-      <c r="E45" s="6" t="n"/>
-      <c r="F45" s="6" t="n"/>
-      <c r="G45" s="6" t="n"/>
-      <c r="H45" s="6" t="n"/>
-      <c r="I45" s="6" t="n"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="6" t="n"/>
-      <c r="B46" s="6" t="n"/>
-      <c r="C46" s="6" t="n"/>
-      <c r="D46" s="6" t="n"/>
-      <c r="E46" s="6" t="n"/>
-      <c r="F46" s="6" t="n"/>
-      <c r="G46" s="6" t="n"/>
-      <c r="H46" s="6" t="n"/>
-      <c r="I46" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -7614,7 +7311,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7629,10 +7326,10 @@
     <row r="1" spans="1:9">
       <c r="A1" s="6" t="n"/>
       <c r="B1" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D1" s="6" t="n"/>
       <c r="E1" s="6" t="n"/>
@@ -7646,10 +7343,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D2" s="6" t="n"/>
       <c r="E2" s="6" t="n"/>
@@ -7663,10 +7360,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D3" s="6" t="n"/>
       <c r="E3" s="6" t="n"/>
@@ -7680,10 +7377,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D4" s="6" t="n"/>
       <c r="E4" s="6" t="n"/>
@@ -7697,10 +7394,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D5" s="6" t="n"/>
       <c r="E5" s="6" t="n"/>
@@ -7714,10 +7411,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D6" s="6" t="n"/>
       <c r="E6" s="6" t="n"/>
@@ -7731,10 +7428,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D7" s="6" t="n"/>
       <c r="E7" s="6" t="n"/>
@@ -7748,10 +7445,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D8" s="6" t="n"/>
       <c r="E8" s="6" t="n"/>
@@ -7765,10 +7462,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D9" s="6" t="n"/>
       <c r="E9" s="6" t="n"/>
@@ -7782,10 +7479,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D10" s="6" t="n"/>
       <c r="E10" s="6" t="n"/>
@@ -7799,10 +7496,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D11" s="6" t="n"/>
       <c r="E11" s="6" t="n"/>
@@ -7816,10 +7513,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D12" s="6" t="n"/>
       <c r="E12" s="6" t="n"/>
@@ -7833,10 +7530,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D13" s="6" t="n"/>
       <c r="E13" s="6" t="n"/>
@@ -7850,10 +7547,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D14" s="6" t="n"/>
       <c r="E14" s="6" t="n"/>
@@ -7867,10 +7564,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D15" s="6" t="n"/>
       <c r="E15" s="6" t="n"/>
@@ -7884,10 +7581,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D16" s="6" t="n"/>
       <c r="E16" s="6" t="n"/>
@@ -7901,10 +7598,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D17" s="6" t="n"/>
       <c r="E17" s="6" t="n"/>
@@ -7918,10 +7615,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D18" s="6" t="n"/>
       <c r="E18" s="6" t="n"/>
@@ -7935,10 +7632,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D19" s="6" t="n"/>
       <c r="E19" s="6" t="n"/>
@@ -7952,10 +7649,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D20" s="6" t="n"/>
       <c r="E20" s="6" t="n"/>
@@ -7969,10 +7666,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D21" s="6" t="n"/>
       <c r="E21" s="6" t="n"/>
@@ -7986,10 +7683,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D22" s="6" t="n"/>
       <c r="E22" s="6" t="n"/>
@@ -8003,10 +7700,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D23" s="6" t="n"/>
       <c r="E23" s="6" t="n"/>
@@ -8020,10 +7717,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D24" s="6" t="n"/>
       <c r="E24" s="6" t="n"/>
@@ -8037,10 +7734,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D25" s="6" t="n"/>
       <c r="E25" s="6" t="n"/>
@@ -8054,10 +7751,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D26" s="6" t="n"/>
       <c r="E26" s="6" t="n"/>
@@ -8071,10 +7768,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D27" s="6" t="n"/>
       <c r="E27" s="6" t="n"/>
@@ -8088,10 +7785,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D28" s="6" t="n"/>
       <c r="E28" s="6" t="n"/>
@@ -8105,10 +7802,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D29" s="6" t="n"/>
       <c r="E29" s="6" t="n"/>
@@ -8122,10 +7819,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D30" s="6" t="n"/>
       <c r="E30" s="6" t="n"/>
@@ -8139,10 +7836,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D31" s="6" t="n"/>
       <c r="E31" s="6" t="n"/>
@@ -8156,10 +7853,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D32" s="6" t="n"/>
       <c r="E32" s="6" t="n"/>
@@ -8173,10 +7870,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D33" s="6" t="n"/>
       <c r="E33" s="6" t="n"/>
@@ -8190,10 +7887,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D34" s="6" t="n"/>
       <c r="E34" s="6" t="n"/>
@@ -8207,10 +7904,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D35" s="6" t="n"/>
       <c r="E35" s="6" t="n"/>
@@ -8220,15 +7917,9 @@
       <c r="I35" s="6" t="n"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="5" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>164</v>
-      </c>
+      <c r="A36" s="6" t="n"/>
+      <c r="B36" s="6" t="n"/>
+      <c r="C36" s="6" t="n"/>
       <c r="D36" s="6" t="n"/>
       <c r="E36" s="6" t="n"/>
       <c r="F36" s="6" t="n"/>
@@ -8237,15 +7928,9 @@
       <c r="I36" s="6" t="n"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>166</v>
-      </c>
+      <c r="A37" s="6" t="n"/>
+      <c r="B37" s="6" t="n"/>
+      <c r="C37" s="6" t="n"/>
       <c r="D37" s="6" t="n"/>
       <c r="E37" s="6" t="n"/>
       <c r="F37" s="6" t="n"/>
@@ -8254,15 +7939,9 @@
       <c r="I37" s="6" t="n"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>168</v>
-      </c>
+      <c r="A38" s="6" t="n"/>
+      <c r="B38" s="6" t="n"/>
+      <c r="C38" s="6" t="n"/>
       <c r="D38" s="6" t="n"/>
       <c r="E38" s="6" t="n"/>
       <c r="F38" s="6" t="n"/>
@@ -8325,39 +8004,6 @@
       <c r="H43" s="6" t="n"/>
       <c r="I43" s="6" t="n"/>
     </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="6" t="n"/>
-      <c r="B44" s="6" t="n"/>
-      <c r="C44" s="6" t="n"/>
-      <c r="D44" s="6" t="n"/>
-      <c r="E44" s="6" t="n"/>
-      <c r="F44" s="6" t="n"/>
-      <c r="G44" s="6" t="n"/>
-      <c r="H44" s="6" t="n"/>
-      <c r="I44" s="6" t="n"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="6" t="n"/>
-      <c r="B45" s="6" t="n"/>
-      <c r="C45" s="6" t="n"/>
-      <c r="D45" s="6" t="n"/>
-      <c r="E45" s="6" t="n"/>
-      <c r="F45" s="6" t="n"/>
-      <c r="G45" s="6" t="n"/>
-      <c r="H45" s="6" t="n"/>
-      <c r="I45" s="6" t="n"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="6" t="n"/>
-      <c r="B46" s="6" t="n"/>
-      <c r="C46" s="6" t="n"/>
-      <c r="D46" s="6" t="n"/>
-      <c r="E46" s="6" t="n"/>
-      <c r="F46" s="6" t="n"/>
-      <c r="G46" s="6" t="n"/>
-      <c r="H46" s="6" t="n"/>
-      <c r="I46" s="6" t="n"/>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>